<commit_message>
premier algo plus ou moins ok. install d'un look and feel
</commit_message>
<xml_diff>
--- a/Excel tests/test droite.xlsx
+++ b/Excel tests/test droite.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +390,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1">
         <v>5</v>
@@ -402,98 +398,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>-2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>-1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
-        <v>6.5</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>